<commit_message>
Chapter 5.1 - Scalability
</commit_message>
<xml_diff>
--- a/src/tables/txs_feedensity_distribution.xlsx
+++ b/src/tables/txs_feedensity_distribution.xlsx
@@ -1,20 +1,33 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="28016"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/enrico/Dropbox/uni/02-master uit/2 - Year/INF-3990 Master Thesis/ete011_rep_code/src/tables/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView activeTab="0"/>
+    <workbookView xWindow="240" yWindow="680" windowWidth="28560" windowHeight="17380"/>
   </bookViews>
   <sheets>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <definedNames/>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+  <calcPr calcId="0" concurrentCalc="0"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
+      <x14:workbookPr defaultImageDpi="32767"/>
+    </ext>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
   <si>
     <t>0 (sat/byte)</t>
   </si>
@@ -70,23 +83,24 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="0"/>
-  <fonts count="2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <color theme="1"/>
-      <sz val="11"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b val="1"/>
+      <b/>
+      <sz val="11"/>
+      <name val="Calibri"/>
     </font>
   </fonts>
   <fills count="2">
     <fill>
-      <patternFill/>
+      <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
@@ -101,27 +115,1451 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin"/>
-      <right style="thin"/>
-      <top style="thin"/>
-      <bottom style="thin"/>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
       <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="2">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf applyAlignment="1" borderId="1" fillId="0" fontId="1" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle builtinId="0" hidden="0" name="Normal" xfId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium9"/>
+  <dxfs count="0"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="stacked"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$B$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>0 (sat/byte)</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:numRef>
+              <c:f>Sheet1!$A$2:$A$10</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>0.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>3.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>4.0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>5.0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>6.0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>7.0</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>8.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$B$2:$B$10</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>201.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>101.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>71.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>70.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>66.0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>220.0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>148.0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>64.0</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>23.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$C$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>&lt;50</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent2"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:numRef>
+              <c:f>Sheet1!$A$2:$A$10</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>0.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>3.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>4.0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>5.0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>6.0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>7.0</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>8.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$C$2:$C$10</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>32050.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>16231.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>15320.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>13205.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2979.0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>20273.0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>68901.0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>57025.0</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>30822.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$D$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>&lt;100</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent3"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:numRef>
+              <c:f>Sheet1!$A$2:$A$10</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>0.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>3.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>4.0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>5.0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>6.0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>7.0</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>8.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$D$2:$D$10</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>229528.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>137037.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>19764.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>19567.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>4839.0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>28727.0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>31252.0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>24335.0</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>10687.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$E$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>&lt;200</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent4"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:numRef>
+              <c:f>Sheet1!$A$2:$A$10</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>0.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>3.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>4.0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>5.0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>6.0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>7.0</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>8.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$E$2:$E$10</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>131002.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>210826.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>253886.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>253845.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>155643.0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>28626.0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>93189.0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>101292.0</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>29566.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="4"/>
+          <c:order val="4"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$F$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>&lt;300</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent5"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:numRef>
+              <c:f>Sheet1!$A$2:$A$10</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>0.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>3.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>4.0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>5.0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>6.0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>7.0</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>8.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$F$2:$F$10</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>6493.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>13642.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>135871.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>77245.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>196235.0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>69707.0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>80514.0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>79118.0</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>22240.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="5"/>
+          <c:order val="5"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$G$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>&gt;300</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent6"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:numRef>
+              <c:f>Sheet1!$A$2:$A$10</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>0.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>3.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>4.0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>5.0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>6.0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>7.0</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>8.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$G$2:$G$10</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>4401.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>8878.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>18061.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>18947.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>136176.0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>231436.0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>62947.0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>112037.0</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>38490.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="150"/>
+        <c:overlap val="100"/>
+        <c:axId val="-2140327520"/>
+        <c:axId val="-2140325472"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="-2140327520"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="-2140325472"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="-2140325472"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="-2140327520"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="297">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>50800</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>63500</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>584200</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>139700</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -408,20 +1846,16 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I10"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="R21" sqref="R21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:9">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
@@ -447,268 +1881,269 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:9">
-      <c r="A2" s="1" t="n">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A2" s="1">
         <v>0</v>
       </c>
-      <c r="B2" t="n">
+      <c r="B2">
         <v>201</v>
       </c>
-      <c r="C2" t="n">
+      <c r="C2">
         <v>32050</v>
       </c>
-      <c r="D2" t="n">
+      <c r="D2">
         <v>229528</v>
       </c>
-      <c r="E2" t="n">
+      <c r="E2">
         <v>131002</v>
       </c>
-      <c r="F2" t="n">
+      <c r="F2">
         <v>6493</v>
       </c>
-      <c r="G2" t="n">
+      <c r="G2">
         <v>4401</v>
       </c>
       <c r="H2" t="s">
         <v>8</v>
       </c>
-      <c r="I2" t="n">
+      <c r="I2">
         <v>403675</v>
       </c>
     </row>
-    <row r="3" spans="1:9">
-      <c r="A3" s="1" t="n">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A3" s="1">
         <v>1</v>
       </c>
-      <c r="B3" t="n">
+      <c r="B3">
         <v>101</v>
       </c>
-      <c r="C3" t="n">
+      <c r="C3">
         <v>16231</v>
       </c>
-      <c r="D3" t="n">
+      <c r="D3">
         <v>137037</v>
       </c>
-      <c r="E3" t="n">
+      <c r="E3">
         <v>210826</v>
       </c>
-      <c r="F3" t="n">
+      <c r="F3">
         <v>13642</v>
       </c>
-      <c r="G3" t="n">
+      <c r="G3">
         <v>8878</v>
       </c>
       <c r="H3" t="s">
         <v>9</v>
       </c>
-      <c r="I3" t="n">
+      <c r="I3">
         <v>386715</v>
       </c>
     </row>
-    <row r="4" spans="1:9">
-      <c r="A4" s="1" t="n">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A4" s="1">
         <v>2</v>
       </c>
-      <c r="B4" t="n">
+      <c r="B4">
         <v>71</v>
       </c>
-      <c r="C4" t="n">
+      <c r="C4">
         <v>15320</v>
       </c>
-      <c r="D4" t="n">
+      <c r="D4">
         <v>19764</v>
       </c>
-      <c r="E4" t="n">
+      <c r="E4">
         <v>253886</v>
       </c>
-      <c r="F4" t="n">
+      <c r="F4">
         <v>135871</v>
       </c>
-      <c r="G4" t="n">
+      <c r="G4">
         <v>18061</v>
       </c>
       <c r="H4" t="s">
         <v>10</v>
       </c>
-      <c r="I4" t="n">
+      <c r="I4">
         <v>442973</v>
       </c>
     </row>
-    <row r="5" spans="1:9">
-      <c r="A5" s="1" t="n">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A5" s="1">
         <v>3</v>
       </c>
-      <c r="B5" t="n">
+      <c r="B5">
         <v>70</v>
       </c>
-      <c r="C5" t="n">
+      <c r="C5">
         <v>13205</v>
       </c>
-      <c r="D5" t="n">
+      <c r="D5">
         <v>19567</v>
       </c>
-      <c r="E5" t="n">
+      <c r="E5">
         <v>253845</v>
       </c>
-      <c r="F5" t="n">
+      <c r="F5">
         <v>77245</v>
       </c>
-      <c r="G5" t="n">
+      <c r="G5">
         <v>18947</v>
       </c>
       <c r="H5" t="s">
         <v>11</v>
       </c>
-      <c r="I5" t="n">
+      <c r="I5">
         <v>382879</v>
       </c>
     </row>
-    <row r="6" spans="1:9">
-      <c r="A6" s="1" t="n">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A6" s="1">
         <v>4</v>
       </c>
-      <c r="B6" t="n">
+      <c r="B6">
         <v>66</v>
       </c>
-      <c r="C6" t="n">
+      <c r="C6">
         <v>2979</v>
       </c>
-      <c r="D6" t="n">
+      <c r="D6">
         <v>4839</v>
       </c>
-      <c r="E6" t="n">
+      <c r="E6">
         <v>155643</v>
       </c>
-      <c r="F6" t="n">
+      <c r="F6">
         <v>196235</v>
       </c>
-      <c r="G6" t="n">
+      <c r="G6">
         <v>136176</v>
       </c>
       <c r="H6" t="s">
         <v>12</v>
       </c>
-      <c r="I6" t="n">
+      <c r="I6">
         <v>495938</v>
       </c>
     </row>
-    <row r="7" spans="1:9">
-      <c r="A7" s="1" t="n">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A7" s="1">
         <v>5</v>
       </c>
-      <c r="B7" t="n">
+      <c r="B7">
         <v>220</v>
       </c>
-      <c r="C7" t="n">
+      <c r="C7">
         <v>20273</v>
       </c>
-      <c r="D7" t="n">
+      <c r="D7">
         <v>28727</v>
       </c>
-      <c r="E7" t="n">
+      <c r="E7">
         <v>28626</v>
       </c>
-      <c r="F7" t="n">
+      <c r="F7">
         <v>69707</v>
       </c>
-      <c r="G7" t="n">
+      <c r="G7">
         <v>231436</v>
       </c>
       <c r="H7" t="s">
         <v>13</v>
       </c>
-      <c r="I7" t="n">
+      <c r="I7">
         <v>378989</v>
       </c>
     </row>
-    <row r="8" spans="1:9">
-      <c r="A8" s="1" t="n">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A8" s="1">
         <v>6</v>
       </c>
-      <c r="B8" t="n">
+      <c r="B8">
         <v>148</v>
       </c>
-      <c r="C8" t="n">
+      <c r="C8">
         <v>68901</v>
       </c>
-      <c r="D8" t="n">
+      <c r="D8">
         <v>31252</v>
       </c>
-      <c r="E8" t="n">
+      <c r="E8">
         <v>93189</v>
       </c>
-      <c r="F8" t="n">
+      <c r="F8">
         <v>80514</v>
       </c>
-      <c r="G8" t="n">
+      <c r="G8">
         <v>62947</v>
       </c>
       <c r="H8" t="s">
         <v>14</v>
       </c>
-      <c r="I8" t="n">
+      <c r="I8">
         <v>336951</v>
       </c>
     </row>
-    <row r="9" spans="1:9">
-      <c r="A9" s="1" t="n">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A9" s="1">
         <v>7</v>
       </c>
-      <c r="B9" t="n">
+      <c r="B9">
         <v>64</v>
       </c>
-      <c r="C9" t="n">
+      <c r="C9">
         <v>57025</v>
       </c>
-      <c r="D9" t="n">
+      <c r="D9">
         <v>24335</v>
       </c>
-      <c r="E9" t="n">
+      <c r="E9">
         <v>101292</v>
       </c>
-      <c r="F9" t="n">
+      <c r="F9">
         <v>79118</v>
       </c>
-      <c r="G9" t="n">
+      <c r="G9">
         <v>112037</v>
       </c>
       <c r="H9" t="s">
         <v>15</v>
       </c>
-      <c r="I9" t="n">
+      <c r="I9">
         <v>373871</v>
       </c>
     </row>
-    <row r="10" spans="1:9">
-      <c r="A10" s="1" t="n">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A10" s="1">
         <v>8</v>
       </c>
-      <c r="B10" t="n">
+      <c r="B10">
         <v>23</v>
       </c>
-      <c r="C10" t="n">
+      <c r="C10">
         <v>30822</v>
       </c>
-      <c r="D10" t="n">
+      <c r="D10">
         <v>10687</v>
       </c>
-      <c r="E10" t="n">
+      <c r="E10">
         <v>29566</v>
       </c>
-      <c r="F10" t="n">
+      <c r="F10">
         <v>22240</v>
       </c>
-      <c r="G10" t="n">
+      <c r="G10">
         <v>38490</v>
       </c>
       <c r="H10" t="s">
         <v>16</v>
       </c>
-      <c r="I10" t="n">
+      <c r="I10">
         <v>131828</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>